<commit_message>
Very sad about the genetic algorithm, uploading tables, models and settings for the algorithm and creating the first method in mutation and parental selection, which is Crossover- Single-Point and Tournament Selection, and evaluating the tables in each chromosome and creating a page to show the best five tables from the algorithm and changing the state of the populations and also knowing the best chromosome from this population
</commit_message>
<xml_diff>
--- a/ملفات الاكسل لمشروع التخرج/subject.xlsx
+++ b/ملفات الاكسل لمشروع التخرج/subject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bit\Desktop\tamplete\final\timetable-pro\ملفات الاكسل لمشروع التخرج\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05AC2CD-9A04-4991-A897-780FDCDEE460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5485CC-F434-4FC9-B1E3-1227A58CFC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="0" windowWidth="9630" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
@@ -1562,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I268"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>